<commit_message>
WARNING! not working code add GameState class refactor code
</commit_message>
<xml_diff>
--- a/docs/Doodle Jump RoadMap.xlsx
+++ b/docs/Doodle Jump RoadMap.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DavidOS\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DavidOS\CLionProjects\doodle-jump\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7350"/>
   </bookViews>
   <sheets>
     <sheet name="Лист" sheetId="1" r:id="rId1"/>
@@ -90,9 +90,6 @@
     <t>Вывод карты на экран</t>
   </si>
   <si>
-    <t>Сдлеать окно меню</t>
-  </si>
-  <si>
     <t xml:space="preserve">Добавить текстуры бонусов </t>
   </si>
   <si>
@@ -114,9 +111,6 @@
     <t>Падать вниз на платформы</t>
   </si>
   <si>
-    <t>Доработать генераторкарт(генерация платформ)</t>
-  </si>
-  <si>
     <t>Пользователь прыгает вверх пока не упадёт ниже экрана</t>
   </si>
   <si>
@@ -166,6 +160,12 @@
   </si>
   <si>
     <t>Бонус "Реактивный ранец"</t>
+  </si>
+  <si>
+    <t>Доработать генератор карт(генерация платформ)</t>
+  </si>
+  <si>
+    <t>Сделать окно меню</t>
   </si>
 </sst>
 </file>
@@ -471,6 +471,48 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -498,50 +540,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -825,8 +825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8:L8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11:J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -859,83 +859,83 @@
     </row>
     <row r="2" spans="1:14" ht="24" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
-      <c r="B2" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="14"/>
+      <c r="B2" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="28"/>
     </row>
     <row r="3" spans="1:14" ht="24" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
-      <c r="M3" s="16"/>
-      <c r="N3" s="17"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="30"/>
+      <c r="M3" s="30"/>
+      <c r="N3" s="31"/>
     </row>
     <row r="4" spans="1:14" ht="24" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-      <c r="M4" s="19"/>
-      <c r="N4" s="20"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
+      <c r="K4" s="33"/>
+      <c r="L4" s="33"/>
+      <c r="M4" s="33"/>
+      <c r="N4" s="34"/>
     </row>
     <row r="5" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="32">
+      <c r="C5" s="14">
         <v>1</v>
       </c>
-      <c r="D5" s="22"/>
-      <c r="E5" s="32">
+      <c r="D5" s="13"/>
+      <c r="E5" s="14">
         <v>2</v>
       </c>
-      <c r="F5" s="22"/>
-      <c r="G5" s="33">
+      <c r="F5" s="13"/>
+      <c r="G5" s="15">
         <v>3</v>
       </c>
-      <c r="H5" s="22"/>
-      <c r="I5" s="34">
+      <c r="H5" s="13"/>
+      <c r="I5" s="17">
         <v>4</v>
       </c>
-      <c r="J5" s="22"/>
-      <c r="K5" s="24">
+      <c r="J5" s="13"/>
+      <c r="K5" s="35">
         <v>5</v>
       </c>
-      <c r="L5" s="22"/>
-      <c r="M5" s="24">
+      <c r="L5" s="13"/>
+      <c r="M5" s="35">
         <v>6</v>
       </c>
-      <c r="N5" s="22"/>
+      <c r="N5" s="13"/>
     </row>
     <row r="6" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
@@ -984,188 +984,188 @@
       <c r="B7" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="21" t="s">
+      <c r="D7" s="13"/>
+      <c r="E7" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="22"/>
-      <c r="G7" s="21" t="s">
+      <c r="F7" s="13"/>
+      <c r="G7" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="H7" s="22"/>
-      <c r="I7" s="21" t="s">
+      <c r="H7" s="13"/>
+      <c r="I7" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="J7" s="22"/>
-      <c r="K7" s="21" t="s">
+      <c r="J7" s="13"/>
+      <c r="K7" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="L7" s="22"/>
-      <c r="M7" s="21" t="s">
+      <c r="L7" s="13"/>
+      <c r="M7" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="N7" s="22"/>
+      <c r="N7" s="13"/>
     </row>
     <row r="8" spans="1:14" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="7"/>
       <c r="B8" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="22"/>
-      <c r="E8" s="25" t="s">
+      <c r="D8" s="13"/>
+      <c r="E8" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="22"/>
-      <c r="G8" s="23" t="s">
+      <c r="F8" s="13"/>
+      <c r="G8" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="13"/>
+      <c r="I8" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="J8" s="13"/>
+      <c r="K8" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="H8" s="22"/>
-      <c r="I8" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="J8" s="22"/>
-      <c r="K8" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="L8" s="22"/>
-      <c r="M8" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="N8" s="22"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="N8" s="13"/>
     </row>
     <row r="9" spans="1:14" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" s="7"/>
       <c r="B9" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="22"/>
-      <c r="E9" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="22"/>
-      <c r="G9" s="23" t="s">
+      <c r="D9" s="13"/>
+      <c r="E9" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="13"/>
+      <c r="G9" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9" s="13"/>
+      <c r="I9" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="J9" s="13"/>
+      <c r="K9" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="H9" s="22"/>
-      <c r="I9" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="J9" s="22"/>
-      <c r="K9" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="L9" s="22"/>
-      <c r="M9" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="N9" s="22"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="N9" s="13"/>
     </row>
     <row r="10" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="7"/>
-      <c r="B10" s="26" t="s">
+      <c r="B10" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="31" t="s">
+      <c r="C10" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="22"/>
-      <c r="E10" s="35" t="s">
+      <c r="D10" s="13"/>
+      <c r="E10" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="22"/>
-      <c r="G10" s="31" t="s">
+      <c r="F10" s="13"/>
+      <c r="G10" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="H10" s="22"/>
-      <c r="I10" s="25" t="s">
+      <c r="H10" s="13"/>
+      <c r="I10" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="J10" s="22"/>
-      <c r="K10" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="L10" s="22"/>
-      <c r="M10" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="N10" s="22"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="L10" s="13"/>
+      <c r="M10" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="N10" s="13"/>
     </row>
     <row r="11" spans="1:14" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7"/>
-      <c r="B11" s="27"/>
-      <c r="C11" s="31" t="s">
+      <c r="B11" s="22"/>
+      <c r="C11" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="22"/>
-      <c r="E11" s="31" t="s">
+      <c r="D11" s="13"/>
+      <c r="E11" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="22"/>
-      <c r="G11" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="H11" s="22"/>
-      <c r="I11" s="25" t="s">
+      <c r="F11" s="13"/>
+      <c r="G11" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="H11" s="13"/>
+      <c r="I11" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="J11" s="13"/>
+      <c r="K11" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="L11" s="13"/>
+      <c r="M11" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="J11" s="22"/>
-      <c r="K11" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="L11" s="22"/>
-      <c r="M11" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="N11" s="22"/>
+      <c r="N11" s="13"/>
     </row>
     <row r="12" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="7"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="J12" s="22"/>
-      <c r="K12" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="L12" s="22"/>
-      <c r="M12" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="N12" s="22"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="J12" s="13"/>
+      <c r="K12" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="L12" s="13"/>
+      <c r="M12" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="N12" s="13"/>
     </row>
     <row r="13" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="7"/>
-      <c r="B13" s="28"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="J13" s="22"/>
-      <c r="K13" s="25"/>
-      <c r="L13" s="22"/>
-      <c r="M13" s="25"/>
-      <c r="N13" s="22"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="J13" s="13"/>
+      <c r="K13" s="20"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="20"/>
+      <c r="N13" s="13"/>
     </row>
     <row r="14" spans="1:14" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A14" s="9"/>
@@ -1178,44 +1178,82 @@
     <row r="16" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
       <c r="B16" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16" s="22"/>
+      <c r="D16" s="13"/>
     </row>
     <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
       <c r="B17" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="D17" s="22"/>
+        <v>40</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="13"/>
     </row>
     <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
       <c r="B18" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="C18" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="D18" s="22"/>
+        <v>42</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" s="13"/>
     </row>
     <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="C19" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="D19" s="22"/>
+        <v>44</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="54">
+    <mergeCell ref="B2:N4"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="G8:H8"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="E5:F5"/>
@@ -1232,44 +1270,6 @@
     <mergeCell ref="I11:J11"/>
     <mergeCell ref="G12:H12"/>
     <mergeCell ref="I12:J12"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="B2:N4"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C7:D7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>